<commit_message>
updated db for the pink 3-piece set
</commit_message>
<xml_diff>
--- a/hivaasproductinventory.xlsx
+++ b/hivaasproductinventory.xlsx
@@ -145,16 +145,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>https://drive.google.com/uc?export=view&amp;id=</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>1kK-ap0j-WEDaFO7rhnjxCSX5YkVmhdr</t>
-    </r>
+    <t>https://drive.google.com/uc?export=view&amp;id=1kK-ap0j-WEDaFO7rhnjxCSX5YkVmhdr8</t>
   </si>
   <si>
     <r>
@@ -704,12 +695,19 @@
     <col customWidth="1" min="3" max="3" width="5.0"/>
     <col customWidth="1" min="4" max="4" width="8.25"/>
     <col customWidth="1" min="5" max="5" width="7.75"/>
-    <col customWidth="1" min="6" max="6" width="68.5"/>
-    <col customWidth="1" min="7" max="7" width="64.25"/>
-    <col customWidth="1" min="8" max="8" width="65.5"/>
-    <col customWidth="1" min="9" max="9" width="64.5"/>
-    <col customWidth="1" min="10" max="10" width="64.13"/>
-    <col customWidth="1" min="18" max="18" width="58.75"/>
+    <col customWidth="1" min="6" max="6" width="68.63"/>
+    <col customWidth="1" min="7" max="7" width="67.13"/>
+    <col customWidth="1" min="8" max="8" width="69.0"/>
+    <col customWidth="1" min="9" max="9" width="67.5"/>
+    <col customWidth="1" min="10" max="10" width="65.75"/>
+    <col customWidth="1" min="11" max="11" width="9.25"/>
+    <col customWidth="1" min="12" max="12" width="9.88"/>
+    <col customWidth="1" min="13" max="13" width="7.38"/>
+    <col customWidth="1" min="14" max="14" width="7.5"/>
+    <col customWidth="1" min="15" max="15" width="8.63"/>
+    <col customWidth="1" min="16" max="16" width="7.75"/>
+    <col customWidth="1" min="17" max="17" width="12.13"/>
+    <col customWidth="1" min="18" max="18" width="60.63"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>